<commit_message>
Update Wifi bootloader prelim CPD 8.xlsx
</commit_message>
<xml_diff>
--- a/Wifi bootloader prelim CPD 8.xlsx
+++ b/Wifi bootloader prelim CPD 8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Neil\Dropbox (Mernok Elektronik)\Software\Booyco HMI Utility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDA10543-3B99-4757-BB16-B99C3DB0CB02}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03371AB-EAB3-4875-AB7B-0C4FD639A5BD}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -778,10 +778,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1106,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AL11" sqref="AL11"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1151,22 +1151,22 @@
       <c r="E1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="32"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="32"/>
-      <c r="S1" s="32"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
+      <c r="S1" s="33"/>
       <c r="T1" s="8"/>
       <c r="U1" s="8"/>
       <c r="V1" s="8"/>
@@ -1308,19 +1308,19 @@
       <c r="AD3" s="8">
         <v>27</v>
       </c>
-      <c r="AE3" s="33">
+      <c r="AE3" s="32">
         <v>28</v>
       </c>
       <c r="AF3" s="8">
         <v>29</v>
       </c>
-      <c r="AG3" s="33">
+      <c r="AG3" s="32">
         <v>30</v>
       </c>
       <c r="AH3" s="8">
         <v>31</v>
       </c>
-      <c r="AI3" s="33">
+      <c r="AI3" s="32">
         <v>32</v>
       </c>
       <c r="AJ3" s="8">

</xml_diff>